<commit_message>
Remade the subsystem code, started vision tracking
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\git\2021-2022-BIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1BFE69-CD59-4B48-84E5-8FDC3094044C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDFD89B-999E-4853-AD65-1F80B727BCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{2E74EACA-0456-45A5-9150-589182898202}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>PORT</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>Left Drive Bottom Front (Drivetrain)</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>vision</t>
+  </si>
+  <si>
+    <t>Vision Sensor</t>
   </si>
 </sst>
 </file>
@@ -479,7 +488,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,6 +582,15 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">

</xml_diff>

<commit_message>
Need to re-tune everything w/ gyro
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\git\2021-2022-BIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE13B0EF-99FB-4823-ACDE-86C568FD137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A0117E-044D-4AD7-A2C9-11955C321305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>PORT</t>
   </si>
@@ -45,33 +45,6 @@
     <t>Motor</t>
   </si>
   <si>
-    <t>l_lift_motor</t>
-  </si>
-  <si>
-    <t>Left-Side Lift</t>
-  </si>
-  <si>
-    <t>r_lift_motor</t>
-  </si>
-  <si>
-    <t>Right-Side Lift</t>
-  </si>
-  <si>
-    <t>conveyor_motor</t>
-  </si>
-  <si>
-    <t>Ring Conveyor</t>
-  </si>
-  <si>
-    <t>Vision</t>
-  </si>
-  <si>
-    <t>vision</t>
-  </si>
-  <si>
-    <t>Vision Sensor</t>
-  </si>
-  <si>
     <t>Distance</t>
   </si>
   <si>
@@ -81,63 +54,6 @@
     <t>Distance Sensor</t>
   </si>
   <si>
-    <t>rdbf</t>
-  </si>
-  <si>
-    <t>Right Drive Bottom Front (Drivetrain)</t>
-  </si>
-  <si>
-    <t>rdtf</t>
-  </si>
-  <si>
-    <t>Right Drive Top Front (Drivetrain)</t>
-  </si>
-  <si>
-    <t>rdbr</t>
-  </si>
-  <si>
-    <t>Right Drive Bottom Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>rdtr</t>
-  </si>
-  <si>
-    <t>Right Drive Top Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>Inertial</t>
-  </si>
-  <si>
-    <t>imu</t>
-  </si>
-  <si>
-    <t>Inertial Measurement Unit</t>
-  </si>
-  <si>
-    <t>ldbr</t>
-  </si>
-  <si>
-    <t>Left Drive Bottom Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>ldtr</t>
-  </si>
-  <si>
-    <t>Left Drive Top Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>ldtf</t>
-  </si>
-  <si>
-    <t>Left Drive Top Front (Drivetrain)</t>
-  </si>
-  <si>
-    <t>ldbf</t>
-  </si>
-  <si>
-    <t>Left Drive Bottom Front (Drivetrain)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -162,21 +78,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>claw_solenoid</t>
-  </si>
-  <si>
-    <t>Pneumatic</t>
-  </si>
-  <si>
-    <t>flaps</t>
-  </si>
-  <si>
-    <t>Pneumatic Solenoid for the front claw</t>
-  </si>
-  <si>
-    <t>Pneumatic Solenoid for the front flaps</t>
-  </si>
-  <si>
     <t>Encoder (1)</t>
   </si>
   <si>
@@ -195,10 +96,22 @@
     <t>Right Custom Encoder</t>
   </si>
   <si>
-    <t>rear_clamp</t>
-  </si>
-  <si>
-    <t>Pneumatic Solenoid for the rear claw</t>
+    <t>Right Rear Motor</t>
+  </si>
+  <si>
+    <t>Right Front Motor</t>
+  </si>
+  <si>
+    <t>Left Rear Motor</t>
+  </si>
+  <si>
+    <t>Left Front Motor</t>
+  </si>
+  <si>
+    <t>Old Gyro</t>
+  </si>
+  <si>
+    <t>3-Wire Gyro</t>
   </si>
 </sst>
 </file>
@@ -555,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,43 +497,16 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -651,28 +537,19 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -684,15 +561,6 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -701,26 +569,14 @@
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -729,40 +585,19 @@
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -771,11 +606,8 @@
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -785,128 +617,95 @@
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed hardware ports and refactored
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\git\2021-2022-BIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE13B0EF-99FB-4823-ACDE-86C568FD137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF9D26-88D7-4763-AEC3-D589736B540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>PORT</t>
   </si>
@@ -57,87 +57,15 @@
     <t>Right-Side Lift</t>
   </si>
   <si>
-    <t>conveyor_motor</t>
-  </si>
-  <si>
-    <t>Ring Conveyor</t>
-  </si>
-  <si>
     <t>Vision</t>
   </si>
   <si>
-    <t>vision</t>
-  </si>
-  <si>
-    <t>Vision Sensor</t>
-  </si>
-  <si>
     <t>Distance</t>
   </si>
   <si>
-    <t>goal_sense</t>
-  </si>
-  <si>
     <t>Distance Sensor</t>
   </si>
   <si>
-    <t>rdbf</t>
-  </si>
-  <si>
-    <t>Right Drive Bottom Front (Drivetrain)</t>
-  </si>
-  <si>
-    <t>rdtf</t>
-  </si>
-  <si>
-    <t>Right Drive Top Front (Drivetrain)</t>
-  </si>
-  <si>
-    <t>rdbr</t>
-  </si>
-  <si>
-    <t>Right Drive Bottom Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>rdtr</t>
-  </si>
-  <si>
-    <t>Right Drive Top Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>Inertial</t>
-  </si>
-  <si>
-    <t>imu</t>
-  </si>
-  <si>
-    <t>Inertial Measurement Unit</t>
-  </si>
-  <si>
-    <t>ldbr</t>
-  </si>
-  <si>
-    <t>Left Drive Bottom Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>ldtr</t>
-  </si>
-  <si>
-    <t>Left Drive Top Rear (Drivetrain)</t>
-  </si>
-  <si>
-    <t>ldtf</t>
-  </si>
-  <si>
-    <t>Left Drive Top Front (Drivetrain)</t>
-  </si>
-  <si>
-    <t>ldbf</t>
-  </si>
-  <si>
-    <t>Left Drive Bottom Front (Drivetrain)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -162,43 +90,64 @@
     <t>H</t>
   </si>
   <si>
-    <t>claw_solenoid</t>
-  </si>
-  <si>
-    <t>Pneumatic</t>
-  </si>
-  <si>
-    <t>flaps</t>
-  </si>
-  <si>
-    <t>Pneumatic Solenoid for the front claw</t>
-  </si>
-  <si>
-    <t>Pneumatic Solenoid for the front flaps</t>
-  </si>
-  <si>
-    <t>Encoder (1)</t>
-  </si>
-  <si>
-    <t>Encoder (2)</t>
-  </si>
-  <si>
-    <t>left_enc</t>
-  </si>
-  <si>
-    <t>right_enc</t>
-  </si>
-  <si>
-    <t>Left Custom Encoder</t>
-  </si>
-  <si>
-    <t>Right Custom Encoder</t>
-  </si>
-  <si>
-    <t>rear_clamp</t>
-  </si>
-  <si>
-    <t>Pneumatic Solenoid for the rear claw</t>
+    <t>lt_drive</t>
+  </si>
+  <si>
+    <t>lf_drive</t>
+  </si>
+  <si>
+    <t>lm_drive</t>
+  </si>
+  <si>
+    <t>lb_drive</t>
+  </si>
+  <si>
+    <t>rt_drive</t>
+  </si>
+  <si>
+    <t>rf_drive</t>
+  </si>
+  <si>
+    <t>rm_drive</t>
+  </si>
+  <si>
+    <t>rb_drive</t>
+  </si>
+  <si>
+    <t>l_feed</t>
+  </si>
+  <si>
+    <t>Left Ring Conveyor</t>
+  </si>
+  <si>
+    <t>r_feed</t>
+  </si>
+  <si>
+    <t>Right Ring Conveyor</t>
+  </si>
+  <si>
+    <t>Solenoid</t>
+  </si>
+  <si>
+    <t>cam</t>
+  </si>
+  <si>
+    <t>Vision sensor</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>front_solenoid</t>
+  </si>
+  <si>
+    <t>rear_solenoid</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>tracking_enc</t>
   </si>
 </sst>
 </file>
@@ -555,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,42 +534,24 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -631,54 +562,87 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -688,10 +652,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -702,10 +663,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -716,41 +674,26 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -758,13 +701,10 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -772,13 +712,10 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -786,127 +723,70 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
         <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decent progress on rush auto
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\git\2021-2022-BIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF9D26-88D7-4763-AEC3-D589736B540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F4EC93-798B-470A-8983-EA54336DDE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>PORT</t>
   </si>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,6 +746,12 @@
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">

</xml_diff>

<commit_message>
Final(tm) version of "full" autonomous
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\git\2021-2022-BIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F4EC93-798B-470A-8983-EA54336DDE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747D46B6-2918-4303-8AEA-7445022F642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>PORT</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>tracking_enc</t>
+  </si>
+  <si>
+    <t>back_cam</t>
+  </si>
+  <si>
+    <t>Vision Sensor</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>rear_switch</t>
   </si>
 </sst>
 </file>
@@ -504,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,6 +559,15 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -782,6 +803,12 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>